<commit_message>
Was added boundary conditions: first and second order derivatives
</commit_message>
<xml_diff>
--- a/Кубические сплайны.xlsx
+++ b/Кубические сплайны.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ноут\Documents\Visual Studio 2019\Projects\CubicSpline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Настольный\Documents\Visual Studio 2019\Projects\CubicSplineInterpolation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16920" windowHeight="6708" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16920" windowHeight="6705"/>
   </bookViews>
   <sheets>
     <sheet name="Интерполяция для параболы" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
   <si>
     <t>x</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Исходные данные</t>
+  </si>
+  <si>
+    <t>Интерплояция: f', f''  заданы</t>
+  </si>
+  <si>
+    <t>Эталон</t>
   </si>
 </sst>
 </file>
@@ -282,7 +288,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="7"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -371,6 +377,234 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1BA6-4884-8C81-A11922C22BAF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Интерполяция для параболы'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Интерплояция: f', f''  заданы</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Интерполяция для параболы'!$G$3:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Интерполяция для параболы'!$H$3:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F91E-4471-8755-CB4C6C414D7C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Интерполяция для параболы'!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Эталон</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Интерполяция для параболы'!$A$15:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Интерполяция для параболы'!$B$15:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F91E-4471-8755-CB4C6C414D7C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2690,16 +2924,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>497205</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>403860</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>451485</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3019,23 +3253,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-2</v>
       </c>
@@ -3048,8 +3285,14 @@
       <c r="E2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -3062,8 +3305,14 @@
       <c r="E3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>-2</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3076,60 +3325,202 @@
       <c r="E4">
         <v>2.14046</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>-1.5</v>
+      </c>
+      <c r="H4">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>-1</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>-0.5</v>
       </c>
       <c r="E6">
         <v>8.6340200000000006E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>-0.5</v>
+      </c>
+      <c r="H6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>0.5</v>
       </c>
       <c r="E8">
         <v>0.27190700000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>1.5</v>
       </c>
       <c r="E10">
         <v>2.3260299999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>1.5</v>
+      </c>
+      <c r="H10">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-2</v>
+      </c>
+      <c r="B15">
+        <f>A15*A15</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-1.5</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ref="B16:B23" si="0">A16*A16</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-1</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-0.5</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.5</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1.5</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -3143,13 +3534,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3157,7 +3548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3171,7 +3562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-2.97</v>
       </c>
@@ -3186,7 +3577,7 @@
         <v>-0.17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-2.64</v>
       </c>
@@ -3201,7 +3592,7 @@
         <v>-0.34693200000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-2.31</v>
       </c>
@@ -3216,7 +3607,7 @@
         <v>-0.48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-1.98</v>
       </c>
@@ -3231,7 +3622,7 @@
         <v>-0.632046</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-1.65</v>
       </c>
@@ -3246,7 +3637,7 @@
         <v>-0.74</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-1.32</v>
       </c>
@@ -3261,7 +3652,7 @@
         <v>-0.83772599999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-0.99</v>
       </c>
@@ -3276,7 +3667,7 @@
         <v>-0.92</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-0.66</v>
       </c>
@@ -3291,7 +3682,7 @@
         <v>-0.97455099999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-0.32</v>
       </c>
@@ -3306,7 +3697,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -3320,7 +3711,7 @@
         <v>-0.99782000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.33</v>
       </c>
@@ -3334,7 +3725,7 @@
         <v>-0.97</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.66</v>
       </c>
@@ -3348,7 +3739,7 @@
         <v>-0.91791800000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.99</v>
       </c>
@@ -3362,7 +3753,7 @@
         <v>-0.84</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.32</v>
       </c>
@@ -3376,7 +3767,7 @@
         <v>-0.73550899999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.65</v>
       </c>
@@ -3390,7 +3781,7 @@
         <v>-0.61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.98</v>
       </c>
@@ -3404,7 +3795,7 @@
         <v>-0.46997100000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2.31</v>
       </c>
@@ -3418,7 +3809,7 @@
         <v>-0.31939099999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2.64</v>
       </c>
@@ -3432,7 +3823,7 @@
         <v>-0.161606</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2.97</v>
       </c>
@@ -3447,7 +3838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D22">
         <v>0.16500000000000001</v>
       </c>
@@ -3455,7 +3846,7 @@
         <v>0.16189500000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D23">
         <v>0.33</v>
       </c>
@@ -3463,7 +3854,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D24">
         <v>0.495</v>
       </c>
@@ -3471,7 +3862,7 @@
         <v>0.47035300000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D25">
         <v>0.66</v>
       </c>
@@ -3479,7 +3870,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>0.82499999999999996</v>
       </c>
@@ -3487,7 +3878,7 @@
         <v>0.73544399999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>0.99</v>
       </c>
@@ -3495,7 +3886,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>1.155</v>
       </c>
@@ -3503,7 +3894,7 @@
         <v>0.91786999999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>1.32</v>
       </c>
@@ -3511,7 +3902,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>1.4850000000000001</v>
       </c>
@@ -3519,7 +3910,7 @@
         <v>0.99807500000000005</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D31">
         <v>1.65</v>
       </c>
@@ -3527,7 +3918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D32">
         <v>1.8149999999999999</v>
       </c>
@@ -3535,7 +3926,7 @@
         <v>0.97358</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>1.98</v>
       </c>
@@ -3543,7 +3934,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>2.145</v>
       </c>
@@ -3551,7 +3942,7 @@
         <v>0.84135700000000002</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>2.31</v>
       </c>
@@ -3559,7 +3950,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36">
         <v>2.4750000000000001</v>
       </c>
@@ -3567,7 +3958,7 @@
         <v>0.61849399999999999</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D37">
         <v>2.64</v>
       </c>
@@ -3575,7 +3966,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38">
         <v>2.8050000000000002</v>
       </c>
@@ -3583,7 +3974,7 @@
         <v>0.32841900000000002</v>
       </c>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>2.97</v>
       </c>

</xml_diff>

<commit_message>
try to interpolate by Hermit spline #1
</commit_message>
<xml_diff>
--- a/Кубические сплайны.xlsx
+++ b/Кубические сплайны.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Настольный\Documents\Visual Studio 2019\Projects\CubicSplineInterpolation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ноут\Documents\Visual Studio 2019\Projects\CubicSpline\CubicSpline\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16920" windowHeight="6705"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16920" windowHeight="6708"/>
   </bookViews>
   <sheets>
     <sheet name="Интерполяция для параболы" sheetId="2" r:id="rId1"/>
@@ -979,7 +979,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1660,7 +1659,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1741,7 +1739,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3255,13 +3252,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3272,7 +3269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>-2</v>
       </c>
@@ -3292,7 +3289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -3312,7 +3309,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3332,7 +3329,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5">
         <v>-1</v>
       </c>
@@ -3346,7 +3343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D6">
         <v>-0.5</v>
       </c>
@@ -3360,7 +3357,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D7">
         <v>0</v>
       </c>
@@ -3374,7 +3371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D8">
         <v>0.5</v>
       </c>
@@ -3388,7 +3385,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D9">
         <v>1</v>
       </c>
@@ -3402,7 +3399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D10">
         <v>1.5</v>
       </c>
@@ -3416,7 +3413,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D11">
         <v>2</v>
       </c>
@@ -3430,12 +3427,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -3443,7 +3440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>-2</v>
       </c>
@@ -3452,7 +3449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>-1.5</v>
       </c>
@@ -3461,7 +3458,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>-1</v>
       </c>
@@ -3470,7 +3467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>-0.5</v>
       </c>
@@ -3479,7 +3476,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -3488,7 +3485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0.5</v>
       </c>
@@ -3497,7 +3494,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -3506,7 +3503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1.5</v>
       </c>
@@ -3515,7 +3512,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -3538,9 +3535,9 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3548,7 +3545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3562,7 +3559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>-2.97</v>
       </c>
@@ -3577,7 +3574,7 @@
         <v>-0.17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>-2.64</v>
       </c>
@@ -3592,7 +3589,7 @@
         <v>-0.34693200000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>-2.31</v>
       </c>
@@ -3607,7 +3604,7 @@
         <v>-0.48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>-1.98</v>
       </c>
@@ -3622,7 +3619,7 @@
         <v>-0.632046</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>-1.65</v>
       </c>
@@ -3637,7 +3634,7 @@
         <v>-0.74</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>-1.32</v>
       </c>
@@ -3652,7 +3649,7 @@
         <v>-0.83772599999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>-0.99</v>
       </c>
@@ -3667,7 +3664,7 @@
         <v>-0.92</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>-0.66</v>
       </c>
@@ -3682,7 +3679,7 @@
         <v>-0.97455099999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>-0.32</v>
       </c>
@@ -3697,7 +3694,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
@@ -3711,7 +3708,7 @@
         <v>-0.99782000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0.33</v>
       </c>
@@ -3725,7 +3722,7 @@
         <v>-0.97</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0.66</v>
       </c>
@@ -3739,7 +3736,7 @@
         <v>-0.91791800000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0.99</v>
       </c>
@@ -3753,7 +3750,7 @@
         <v>-0.84</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1.32</v>
       </c>
@@ -3767,7 +3764,7 @@
         <v>-0.73550899999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1.65</v>
       </c>
@@ -3781,7 +3778,7 @@
         <v>-0.61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1.98</v>
       </c>
@@ -3795,7 +3792,7 @@
         <v>-0.46997100000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2.31</v>
       </c>
@@ -3809,7 +3806,7 @@
         <v>-0.31939099999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2.64</v>
       </c>
@@ -3823,7 +3820,7 @@
         <v>-0.161606</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2.97</v>
       </c>
@@ -3838,7 +3835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D22">
         <v>0.16500000000000001</v>
       </c>
@@ -3846,7 +3843,7 @@
         <v>0.16189500000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D23">
         <v>0.33</v>
       </c>
@@ -3854,7 +3851,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D24">
         <v>0.495</v>
       </c>
@@ -3862,7 +3859,7 @@
         <v>0.47035300000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D25">
         <v>0.66</v>
       </c>
@@ -3870,7 +3867,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D26">
         <v>0.82499999999999996</v>
       </c>
@@ -3878,7 +3875,7 @@
         <v>0.73544399999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D27">
         <v>0.99</v>
       </c>
@@ -3886,7 +3883,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D28">
         <v>1.155</v>
       </c>
@@ -3894,7 +3891,7 @@
         <v>0.91786999999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D29">
         <v>1.32</v>
       </c>
@@ -3902,7 +3899,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D30">
         <v>1.4850000000000001</v>
       </c>
@@ -3910,7 +3907,7 @@
         <v>0.99807500000000005</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D31">
         <v>1.65</v>
       </c>
@@ -3918,7 +3915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D32">
         <v>1.8149999999999999</v>
       </c>
@@ -3926,7 +3923,7 @@
         <v>0.97358</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D33">
         <v>1.98</v>
       </c>
@@ -3934,7 +3931,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D34">
         <v>2.145</v>
       </c>
@@ -3942,7 +3939,7 @@
         <v>0.84135700000000002</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D35">
         <v>2.31</v>
       </c>
@@ -3950,7 +3947,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D36">
         <v>2.4750000000000001</v>
       </c>
@@ -3958,7 +3955,7 @@
         <v>0.61849399999999999</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D37">
         <v>2.64</v>
       </c>
@@ -3966,7 +3963,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D38">
         <v>2.8050000000000002</v>
       </c>
@@ -3974,7 +3971,7 @@
         <v>0.32841900000000002</v>
       </c>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D39">
         <v>2.97</v>
       </c>

</xml_diff>

<commit_message>
fix of weights calculating, change default value
</commit_message>
<xml_diff>
--- a/Кубические сплайны.xlsx
+++ b/Кубические сплайны.xlsx
@@ -98,11 +98,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2615,15 +2616,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Интерполяция Эрмита'!$E$21</c:f>
+              <c:f>'Интерполяция Эрмита'!$H$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Немонотонная интерполяция</c:v>
+                  <c:v>Монотонная интерполяция</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2640,302 +2641,13 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="00B0F0"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Интерполяция Эрмита'!$E$23:$E$60</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="38"/>
-                <c:pt idx="0">
-                  <c:v>7.99</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.0400000000000009</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.0900000000000016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.1400000000000023</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.1900000000000031</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.2400000000000038</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.2900000000000045</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.3400000000000052</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.3900000000000059</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.4400000000000066</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.4900000000000073</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.540000000000008</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8.5900000000000087</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8.6400000000000095</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>8.6900000000000102</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8.7400000000000109</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8.7900000000000116</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8.8400000000000123</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8.890000000000013</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>8.9400000000000137</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>8.9900000000000144</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9.0400000000000151</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9.0900000000000158</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9.1400000000000166</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>9.1900000000000173</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>9.6</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Интерполяция Эрмита'!$F$23:$F$60</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="38"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2.94392E-3</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>2.76E-5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.8806699999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.3700000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.5171199999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.2068500000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.5335900000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.00">
-                  <c:v>0.105918</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.114758</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.12280099999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.130991</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.14027200000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.151588</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.165883</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.18398400000000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.20583699999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.23099900000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.25902399999999998</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.289464</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.32187399999999999</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.35580699999999998</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.39081700000000003</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.42645699999999997</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.462281</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.46942800000000001</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.73731800000000003</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.94374000000000002</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.0987899999999999</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.99863599999999997</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.94562400000000002</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.961982</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.99991600000000003</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1.02091</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.0235399999999999</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1.01569</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1.00522</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.99999400000000005</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B8BF-4869-BA9A-BC97E9750425}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Интерполяция Эрмита'!$H$21</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Монотонная интерполяция</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="bg1">
                   <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
+                  <a:schemeClr val="bg1">
                     <a:lumMod val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
@@ -3076,97 +2788,97 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.7904599999999999E-6</c:v>
+                  <c:v>9.9768400000000002E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.76E-5</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>1.9760699999999999E-2</c:v>
+                  <c:v>1.4571300000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
                   <c:v>4.3700000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>5.2170899999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.0">
-                  <c:v>6.0838200000000002E-2</c:v>
+                  <c:v>6.9543400000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>8.9413900000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>6.99346E-2</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.00">
-                  <c:v>7.9693200000000006E-2</c:v>
+                  <c:v>0.10442</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>0.11566899999999999</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>9.0346700000000002E-2</c:v>
+                  <c:v>0.12427000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>0.102128</c:v>
+                  <c:v>0.131332</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>0.11527</c:v>
+                  <c:v>0.137961</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>0.13000600000000001</c:v>
+                  <c:v>0.14526700000000001</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>0.146569</c:v>
+                  <c:v>0.154358</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>0.165191</c:v>
+                  <c:v>0.16634199999999999</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>0.18607599999999999</c:v>
+                  <c:v>0.182203</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>0.20921000000000001</c:v>
+                  <c:v>0.20201</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>0.234482</c:v>
+                  <c:v>0.22542400000000001</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>0.26178000000000001</c:v>
+                  <c:v>0.25210100000000002</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="General">
-                  <c:v>0.29099199999999997</c:v>
+                  <c:v>0.28169899999999998</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="General">
-                  <c:v>0.32200699999999999</c:v>
+                  <c:v>0.31387399999999999</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="General">
-                  <c:v>0.35471200000000003</c:v>
+                  <c:v>0.34828500000000001</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="General">
-                  <c:v>0.38899600000000001</c:v>
+                  <c:v>0.38458799999999999</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="General">
-                  <c:v>0.42474699999999999</c:v>
+                  <c:v>0.42244100000000001</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="General">
-                  <c:v>0.46185399999999999</c:v>
+                  <c:v>0.46150099999999999</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="General">
                   <c:v>0.46942800000000001</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="General">
-                  <c:v>0.77621700000000005</c:v>
+                  <c:v>0.77974500000000002</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="General">
                   <c:v>0.94374000000000002</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="General">
-                  <c:v>0.98688100000000001</c:v>
+                  <c:v>0.98666900000000002</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="General">
                   <c:v>0.99863599999999997</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="General">
-                  <c:v>0.99930300000000005</c:v>
+                  <c:v>0.99930600000000003</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="General">
-                  <c:v>0.99974300000000005</c:v>
+                  <c:v>0.99974499999999999</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="General">
                   <c:v>0.99991600000000003</c:v>
@@ -3206,6 +2918,319 @@
         </c:dLbls>
         <c:axId val="2110257183"/>
         <c:axId val="2110261343"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Интерполяция Эрмита'!$E$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Немонотонная интерполяция</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="00B0F0"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:srgbClr val="00B0F0"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Интерполяция Эрмита'!$E$23:$E$60</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="38"/>
+                      <c:pt idx="0">
+                        <c:v>7.99</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>8.0400000000000009</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>8.0900000000000016</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>8.1400000000000023</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>8.1900000000000031</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>8.2400000000000038</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>8.2900000000000045</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8.3400000000000052</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8.3900000000000059</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>8.4400000000000066</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>8.4900000000000073</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>8.540000000000008</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>8.5900000000000087</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>8.6400000000000095</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>8.6900000000000102</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>8.7400000000000109</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>8.7900000000000116</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>8.8400000000000123</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>8.890000000000013</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>8.9400000000000137</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>8.9900000000000144</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>9.0400000000000151</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>9.0900000000000158</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>9.1400000000000166</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>9.1900000000000173</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>9.1999999999999993</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>9.6</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>20</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Интерполяция Эрмита'!$F$23:$F$60</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="38"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-2.94392E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="2" formatCode="0.00E+00">
+                        <c:v>2.76E-5</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.8806699999999999E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4.3700000000000003E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6.5171199999999999E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>8.2068500000000003E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>9.5335900000000001E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="8" formatCode="0.00">
+                        <c:v>0.105918</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.114758</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.12280099999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.130991</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.14027200000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.151588</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.165883</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.18398400000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.20583699999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.23099900000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.25902399999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.289464</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.32187399999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.35580699999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0.39081700000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.42645699999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0.462281</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>0.46942800000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>0.73731800000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>0.94374000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>1.0987899999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>0.99863599999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>0.94562400000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>0.961982</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>0.99991600000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>1.02091</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>1.0235399999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>1.01569</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>1.00522</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0.99999400000000005</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-B8BF-4869-BA9A-BC97E9750425}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="2110257183"/>
@@ -3566,253 +3591,6 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Интерполяция Эрмита'!$D$64</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Немонотонная интерполяция</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="00B0F0"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Интерполяция Эрмита'!$D$66:$D$96</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>13.5</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>14.5</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>15</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Интерполяция Эрмита'!$E$66:$E$96</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.99925</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.9980100000000007</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.9977599999999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10.0037</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.9830500000000004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.9657300000000006</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.9655400000000007</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>10.0563</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9.7391400000000008</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9.4717599999999997</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9.4685000000000006</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>10.9307</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7.5282799999999996</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.7840100000000003</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>6.0227300000000001</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>32.822299999999998</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>57.371000000000002</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>57.680300000000003</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>56.6494</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>71.237099999999998</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>85</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AB39-429E-B9D4-9F17FF7A57F7}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
@@ -3960,55 +3738,55 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9998799999999992</c:v>
+                  <c:v>9.9998699999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9996700000000001</c:v>
+                  <c:v>9.9996500000000008</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.9996299999999998</c:v>
+                  <c:v>9.9995999999999992</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.0006</c:v>
+                  <c:v>10.0007</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.9971599999999992</c:v>
+                  <c:v>9.9969999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.9942600000000006</c:v>
+                  <c:v>9.9939300000000006</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.9942299999999999</c:v>
+                  <c:v>9.9938900000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.009399999999999</c:v>
+                  <c:v>10.01</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.9562799999999996</c:v>
+                  <c:v>9.9537600000000008</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.9114799999999992</c:v>
+                  <c:v>9.9063700000000008</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.9109300000000005</c:v>
+                  <c:v>9.9057899999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.2164</c:v>
+                  <c:v>10.225300000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>10.5</c:v>
@@ -4017,34 +3795,34 @@
                   <c:v>10.773300000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.320499999999999</c:v>
+                  <c:v>11.3475</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12.5825</c:v>
+                  <c:v>12.6229</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>32.551600000000001</c:v>
+                  <c:v>31.851700000000001</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>52.307000000000002</c:v>
+                  <c:v>54.0274</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>54.049500000000002</c:v>
+                  <c:v>55.918700000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>56.267299999999999</c:v>
+                  <c:v>57.3506</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>70.584199999999996</c:v>
+                  <c:v>70.329300000000003</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>85</c:v>
@@ -4069,6 +3847,277 @@
         </c:dLbls>
         <c:axId val="213088815"/>
         <c:axId val="213083823"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Интерполяция Эрмита'!$D$64</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Немонотонная интерполяция</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="00B0F0"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:srgbClr val="00B0F0"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Интерполяция Эрмита'!$D$66:$D$96</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="31"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.5</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4.5</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>5.5</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>6.5</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>7.5</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>8.5</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>9.5</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>10.5</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>11.5</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>12.5</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>13.5</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>14.5</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>15</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Интерполяция Эрмита'!$E$66:$E$96</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="31"/>
+                      <c:pt idx="0">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>9.99925</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>9.9980100000000007</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>9.9977599999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>10.0037</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>9.9830500000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>9.9657300000000006</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>9.9655400000000007</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>10.0563</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>9.7391400000000008</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>9.4717599999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>9.4685000000000006</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>10.9307</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>10.5</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>7.5282799999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>4.7840100000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>6.0227300000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>32.822299999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>57.371000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>57.680300000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>56.6494</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>71.237099999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>85</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-AB39-429E-B9D4-9F17FF7A57F7}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="213088815"/>
@@ -4423,313 +4472,6 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Интерполяция Эрмита'!$D$99</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Немонотонная интерполяция</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="00B0F0"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Интерполяция Эрмита'!$D$101:$D$141</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.75</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.25</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.25</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.75</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>5.25</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5.75</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6.25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>6.75</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7.25</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>7.75</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>8.25</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>8.75</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>9.25</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>9.75</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Интерполяция Эрмита'!$E$101:$E$141</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.6568299999999994</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.4182100000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.9704800000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.4658600000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.14595</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.83907</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.8626499999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.07341</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.0611300000000004</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.98041</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.84849</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.6825999999999999</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.3487200000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.7985099999999998</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.45946</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>5.2406800000000002</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>6.6222200000000004</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7.1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>7.4528100000000004</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>7.6995100000000001</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>7.8588300000000002</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>7.9494999999999996</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7.9902199999999999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>7.9997400000000001</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>7.9967499999999996</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>8.0243000000000002</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>8.0688600000000008</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>8.1290200000000006</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>8.2001000000000008</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>8.2774099999999997</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>8.3562899999999996</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>8.4320400000000006</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>8.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-966F-4DCF-8A4F-5C6D846A360A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
@@ -4907,121 +4649,121 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.5046700000000008</c:v>
+                  <c:v>9.6563099999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.0124399999999998</c:v>
+                  <c:v>9.4168199999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.5139999999999993</c:v>
+                  <c:v>8.9689200000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.5361799999999999</c:v>
+                  <c:v>6.3121600000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.4801799999999998</c:v>
+                  <c:v>4.5323200000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.2000900000000003</c:v>
+                  <c:v>4.2517899999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0699500000000004</c:v>
+                  <c:v>4.0953799999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.9216299999999999</c:v>
+                  <c:v>3.9136299999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.83114</c:v>
+                  <c:v>3.8270200000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.7361300000000002</c:v>
+                  <c:v>3.74125</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.6442100000000002</c:v>
+                  <c:v>3.6574300000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.5629599999999999</c:v>
+                  <c:v>3.5766399999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.4490400000000001</c:v>
+                  <c:v>3.4331499999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.63462</c:v>
+                  <c:v>3.6513</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.2897800000000004</c:v>
+                  <c:v>4.2935999999999996</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.1500500000000002</c:v>
+                  <c:v>5.1391099999999996</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6.6895100000000003</c:v>
+                  <c:v>6.6988799999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.29643</c:v>
+                  <c:v>7.2929199999999996</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.4590699999999996</c:v>
+                  <c:v>7.4537800000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.5928300000000002</c:v>
+                  <c:v>7.58711</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.70261</c:v>
+                  <c:v>7.6974600000000004</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.79331</c:v>
+                  <c:v>7.78939</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.8698399999999999</c:v>
+                  <c:v>7.8674200000000001</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.9371</c:v>
+                  <c:v>7.9361100000000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.0623799999999992</c:v>
+                  <c:v>8.0628899999999994</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.1248299999999993</c:v>
+                  <c:v>8.1255699999999997</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8.1873199999999997</c:v>
+                  <c:v>8.1880900000000008</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.2498500000000003</c:v>
+                  <c:v>8.2505100000000002</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8.3123900000000006</c:v>
+                  <c:v>8.3128600000000006</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>8.3749400000000005</c:v>
+                  <c:v>8.3751899999999999</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.4374800000000008</c:v>
+                  <c:v>8.4375599999999995</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>8.5</c:v>
@@ -5046,6 +4788,337 @@
         </c:dLbls>
         <c:axId val="213088815"/>
         <c:axId val="213083823"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Интерполяция Эрмита'!$D$99</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Немонотонная интерполяция</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="00B0F0"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:srgbClr val="00B0F0"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Интерполяция Эрмита'!$D$101:$D$141</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="41"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.25</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.75</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.25</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1.75</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2.25</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>2.5</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>2.75</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>3.25</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>3.5</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>3.75</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>4.25</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>4.5</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>4.75</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>5.25</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>5.5</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>5.75</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>6.25</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>6.5</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>6.75</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>7.25</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>7.5</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>7.75</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>8.25</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>8.5</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>8.75</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>9.25</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>9.5</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>9.75</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>10</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Интерполяция Эрмита'!$E$101:$E$141</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="41"/>
+                      <c:pt idx="0">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>9.6568299999999994</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>9.4182100000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>8.9704800000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6.4658600000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>4.14595</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3.83907</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>3.8626499999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>4.07341</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>4.0611300000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>3.98041</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>3.84849</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>3.6825999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>3.5</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>3.3487200000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>3.4</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>3.7985099999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>4.45946</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>5.2406800000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>6.6222200000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>7.1</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>7.4528100000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>7.6995100000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>7.8588300000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>7.9494999999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>7.9902199999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>7.9997400000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>7.9967499999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>8.0243000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>8.0688600000000008</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>8.1290200000000006</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>8.2001000000000008</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>8.2774099999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>8.3562899999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>8.4320400000000006</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>8.5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-966F-4DCF-8A4F-5C6D846A360A}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="213088815"/>
@@ -8688,16 +8761,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8718,16 +8791,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8748,16 +8821,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>98</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>124</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9781,10 +9854,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X141"/>
+  <dimension ref="A1:AZ141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="K70" sqref="K70"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10096,7 +10169,7 @@
         <v>8.0399999999999991</v>
       </c>
       <c r="I24" s="3">
-        <v>7.7904599999999999E-6</v>
+        <v>9.9768400000000002E-6</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -10144,7 +10217,7 @@
         <v>8.14</v>
       </c>
       <c r="I26">
-        <v>1.9760699999999999E-2</v>
+        <v>1.4571300000000001E-2</v>
       </c>
       <c r="J26" s="3"/>
       <c r="L26" s="3"/>
@@ -10190,7 +10263,7 @@
         <v>8.24</v>
       </c>
       <c r="I28">
-        <v>5.2170899999999999E-2</v>
+        <v>6.9543400000000005E-2</v>
       </c>
       <c r="J28" s="3"/>
       <c r="L28" s="3"/>
@@ -10212,12 +10285,11 @@
       <c r="H29">
         <v>8.2899999999999991</v>
       </c>
-      <c r="I29" s="2">
-        <v>6.0838200000000002E-2</v>
+      <c r="I29">
+        <v>8.9413900000000004E-2</v>
       </c>
       <c r="J29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="2"/>
       <c r="N29" s="2"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.3">
@@ -10238,7 +10310,7 @@
         <v>8.34</v>
       </c>
       <c r="I30">
-        <v>6.99346E-2</v>
+        <v>0.10442</v>
       </c>
       <c r="J30" s="3"/>
       <c r="L30" s="3"/>
@@ -10260,12 +10332,11 @@
       <c r="H31" s="1">
         <v>8.39</v>
       </c>
-      <c r="I31" s="1">
-        <v>7.9693200000000006E-2</v>
+      <c r="I31">
+        <v>0.11566899999999999</v>
       </c>
       <c r="J31" s="3"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -10290,7 +10361,7 @@
         <v>8.44</v>
       </c>
       <c r="I32">
-        <v>9.0346700000000002E-2</v>
+        <v>0.12427000000000001</v>
       </c>
       <c r="J32" s="3"/>
       <c r="L32" s="3"/>
@@ -10307,7 +10378,7 @@
         <v>8.49</v>
       </c>
       <c r="I33">
-        <v>0.102128</v>
+        <v>0.131332</v>
       </c>
       <c r="J33" s="3"/>
       <c r="L33" s="3"/>
@@ -10324,7 +10395,7 @@
         <v>8.5399999999999991</v>
       </c>
       <c r="I34">
-        <v>0.11527</v>
+        <v>0.137961</v>
       </c>
       <c r="J34" s="3"/>
       <c r="L34" s="3"/>
@@ -10341,7 +10412,7 @@
         <v>8.59</v>
       </c>
       <c r="I35">
-        <v>0.13000600000000001</v>
+        <v>0.14526700000000001</v>
       </c>
       <c r="J35" s="3"/>
       <c r="L35" s="3"/>
@@ -10358,7 +10429,7 @@
         <v>8.64</v>
       </c>
       <c r="I36">
-        <v>0.146569</v>
+        <v>0.154358</v>
       </c>
       <c r="J36" s="3"/>
       <c r="L36" s="3"/>
@@ -10375,7 +10446,7 @@
         <v>8.69</v>
       </c>
       <c r="I37">
-        <v>0.165191</v>
+        <v>0.16634199999999999</v>
       </c>
       <c r="J37" s="3"/>
       <c r="L37" s="3"/>
@@ -10392,7 +10463,7 @@
         <v>8.74</v>
       </c>
       <c r="I38">
-        <v>0.18607599999999999</v>
+        <v>0.182203</v>
       </c>
       <c r="J38" s="3"/>
       <c r="L38" s="3"/>
@@ -10409,7 +10480,7 @@
         <v>8.7899999999999991</v>
       </c>
       <c r="I39">
-        <v>0.20921000000000001</v>
+        <v>0.20201</v>
       </c>
       <c r="J39" s="3"/>
       <c r="L39" s="3"/>
@@ -10426,7 +10497,7 @@
         <v>8.84</v>
       </c>
       <c r="I40">
-        <v>0.234482</v>
+        <v>0.22542400000000001</v>
       </c>
       <c r="J40" s="3"/>
       <c r="L40" s="3"/>
@@ -10443,7 +10514,7 @@
         <v>8.89</v>
       </c>
       <c r="I41">
-        <v>0.26178000000000001</v>
+        <v>0.25210100000000002</v>
       </c>
       <c r="J41" s="3"/>
       <c r="L41" s="3"/>
@@ -10460,7 +10531,7 @@
         <v>8.94</v>
       </c>
       <c r="I42">
-        <v>0.29099199999999997</v>
+        <v>0.28169899999999998</v>
       </c>
       <c r="J42" s="3"/>
       <c r="L42" s="3"/>
@@ -10477,7 +10548,7 @@
         <v>8.99</v>
       </c>
       <c r="I43">
-        <v>0.32200699999999999</v>
+        <v>0.31387399999999999</v>
       </c>
       <c r="J43" s="3"/>
       <c r="L43" s="3"/>
@@ -10494,7 +10565,7 @@
         <v>9.0399999999999991</v>
       </c>
       <c r="I44">
-        <v>0.35471200000000003</v>
+        <v>0.34828500000000001</v>
       </c>
       <c r="J44" s="3"/>
       <c r="L44" s="3"/>
@@ -10511,7 +10582,7 @@
         <v>9.09</v>
       </c>
       <c r="I45">
-        <v>0.38899600000000001</v>
+        <v>0.38458799999999999</v>
       </c>
       <c r="J45" s="3"/>
       <c r="L45" s="3"/>
@@ -10528,7 +10599,7 @@
         <v>9.14</v>
       </c>
       <c r="I46">
-        <v>0.42474699999999999</v>
+        <v>0.42244100000000001</v>
       </c>
       <c r="J46" s="3"/>
       <c r="L46" s="3"/>
@@ -10545,7 +10616,7 @@
         <v>9.19</v>
       </c>
       <c r="I47">
-        <v>0.46185399999999999</v>
+        <v>0.46150099999999999</v>
       </c>
       <c r="J47" s="3"/>
       <c r="L47" s="3"/>
@@ -10578,7 +10649,7 @@
         <v>9.6</v>
       </c>
       <c r="I49">
-        <v>0.77621700000000005</v>
+        <v>0.77974500000000002</v>
       </c>
       <c r="J49" s="3"/>
       <c r="L49" s="3"/>
@@ -10611,7 +10682,7 @@
         <v>11</v>
       </c>
       <c r="I51">
-        <v>0.98688100000000001</v>
+        <v>0.98666900000000002</v>
       </c>
       <c r="J51" s="3"/>
       <c r="L51" s="3"/>
@@ -10645,7 +10716,7 @@
         <v>13</v>
       </c>
       <c r="I53">
-        <v>0.99930300000000005</v>
+        <v>0.99930600000000003</v>
       </c>
       <c r="J53" s="3"/>
       <c r="L53" s="3"/>
@@ -10662,7 +10733,7 @@
         <v>14</v>
       </c>
       <c r="I54">
-        <v>0.99974300000000005</v>
+        <v>0.99974499999999999</v>
       </c>
       <c r="J54" s="3"/>
       <c r="L54" s="3"/>
@@ -10769,6 +10840,9 @@
       <c r="J60" s="3"/>
       <c r="L60" s="3"/>
     </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L61" s="3"/>
+    </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>9</v>
@@ -10837,7 +10911,7 @@
         <v>0.5</v>
       </c>
       <c r="H67">
-        <v>9.9998799999999992</v>
+        <v>9.9998699999999996</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -10857,7 +10931,7 @@
         <v>1</v>
       </c>
       <c r="H68">
-        <v>9.9996700000000001</v>
+        <v>9.9996500000000008</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
@@ -10877,7 +10951,7 @@
         <v>1.5</v>
       </c>
       <c r="H69">
-        <v>9.9996299999999998</v>
+        <v>9.9995999999999992</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
@@ -10901,7 +10975,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A71">
+      <c r="A71" s="4">
         <v>8</v>
       </c>
       <c r="B71">
@@ -10917,11 +10991,11 @@
         <v>2.5</v>
       </c>
       <c r="H71">
-        <v>10.0006</v>
+        <v>10.0007</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A72">
+      <c r="A72" s="4">
         <v>9</v>
       </c>
       <c r="B72">
@@ -10941,7 +11015,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A73">
+      <c r="A73" s="4">
         <v>11</v>
       </c>
       <c r="B73">
@@ -10957,11 +11031,11 @@
         <v>3.5</v>
       </c>
       <c r="H73">
-        <v>9.9971599999999992</v>
+        <v>9.9969999999999999</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74">
+      <c r="A74" s="4">
         <v>12</v>
       </c>
       <c r="B74">
@@ -10977,11 +11051,11 @@
         <v>4</v>
       </c>
       <c r="H74">
-        <v>9.9942600000000006</v>
+        <v>9.9939300000000006</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A75">
+      <c r="A75" s="4">
         <v>14</v>
       </c>
       <c r="B75">
@@ -10997,11 +11071,11 @@
         <v>4.5</v>
       </c>
       <c r="H75">
-        <v>9.9942299999999999</v>
+        <v>9.9938900000000004</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A76">
+      <c r="A76" s="4">
         <v>15</v>
       </c>
       <c r="B76">
@@ -11031,7 +11105,7 @@
         <v>5.5</v>
       </c>
       <c r="H77">
-        <v>10.009399999999999</v>
+        <v>10.01</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
@@ -11059,7 +11133,7 @@
         <v>6.5</v>
       </c>
       <c r="H79">
-        <v>9.9562799999999996</v>
+        <v>9.9537600000000008</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
@@ -11073,7 +11147,7 @@
         <v>7</v>
       </c>
       <c r="H80">
-        <v>9.9114799999999992</v>
+        <v>9.9063700000000008</v>
       </c>
     </row>
     <row r="81" spans="4:8" x14ac:dyDescent="0.3">
@@ -11087,7 +11161,7 @@
         <v>7.5</v>
       </c>
       <c r="H81">
-        <v>9.9109300000000005</v>
+        <v>9.9057899999999997</v>
       </c>
     </row>
     <row r="82" spans="4:8" x14ac:dyDescent="0.3">
@@ -11115,7 +11189,7 @@
         <v>8.5</v>
       </c>
       <c r="H83">
-        <v>10.2164</v>
+        <v>10.225300000000001</v>
       </c>
     </row>
     <row r="84" spans="4:8" x14ac:dyDescent="0.3">
@@ -11157,7 +11231,7 @@
         <v>10</v>
       </c>
       <c r="H86">
-        <v>11.320499999999999</v>
+        <v>11.3475</v>
       </c>
     </row>
     <row r="87" spans="4:8" x14ac:dyDescent="0.3">
@@ -11171,7 +11245,7 @@
         <v>10.5</v>
       </c>
       <c r="H87">
-        <v>12.5825</v>
+        <v>12.6229</v>
       </c>
     </row>
     <row r="88" spans="4:8" x14ac:dyDescent="0.3">
@@ -11199,7 +11273,7 @@
         <v>11.5</v>
       </c>
       <c r="H89">
-        <v>32.551600000000001</v>
+        <v>31.851700000000001</v>
       </c>
     </row>
     <row r="90" spans="4:8" x14ac:dyDescent="0.3">
@@ -11227,7 +11301,7 @@
         <v>12.5</v>
       </c>
       <c r="H91">
-        <v>52.307000000000002</v>
+        <v>54.0274</v>
       </c>
     </row>
     <row r="92" spans="4:8" x14ac:dyDescent="0.3">
@@ -11241,7 +11315,7 @@
         <v>13</v>
       </c>
       <c r="H92">
-        <v>54.049500000000002</v>
+        <v>55.918700000000001</v>
       </c>
     </row>
     <row r="93" spans="4:8" x14ac:dyDescent="0.3">
@@ -11255,7 +11329,7 @@
         <v>13.5</v>
       </c>
       <c r="H93">
-        <v>56.267299999999999</v>
+        <v>57.3506</v>
       </c>
     </row>
     <row r="94" spans="4:8" x14ac:dyDescent="0.3">
@@ -11283,7 +11357,7 @@
         <v>14.5</v>
       </c>
       <c r="H95">
-        <v>70.584199999999996</v>
+        <v>70.329300000000003</v>
       </c>
     </row>
     <row r="96" spans="4:8" x14ac:dyDescent="0.3">
@@ -11368,7 +11442,7 @@
         <v>0.25</v>
       </c>
       <c r="H102">
-        <v>9.5046700000000008</v>
+        <v>9.6563099999999995</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
@@ -11388,7 +11462,7 @@
         <v>0.5</v>
       </c>
       <c r="H103">
-        <v>9.0124399999999998</v>
+        <v>9.4168199999999995</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
@@ -11408,7 +11482,7 @@
         <v>0.75</v>
       </c>
       <c r="H104">
-        <v>8.5139999999999993</v>
+        <v>8.9689200000000007</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
@@ -11448,7 +11522,7 @@
         <v>1.25</v>
       </c>
       <c r="H106">
-        <v>6.5361799999999999</v>
+        <v>6.3121600000000004</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
@@ -11488,7 +11562,7 @@
         <v>1.75</v>
       </c>
       <c r="H108">
-        <v>4.4801799999999998</v>
+        <v>4.5323200000000003</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
@@ -11508,7 +11582,7 @@
         <v>2</v>
       </c>
       <c r="H109">
-        <v>4.2000900000000003</v>
+        <v>4.2517899999999997</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
@@ -11528,7 +11602,7 @@
         <v>2.25</v>
       </c>
       <c r="H110">
-        <v>4.0699500000000004</v>
+        <v>4.0953799999999996</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
@@ -11556,10 +11630,10 @@
         <v>2.75</v>
       </c>
       <c r="H112">
-        <v>3.9216299999999999</v>
-      </c>
-    </row>
-    <row r="113" spans="4:8" x14ac:dyDescent="0.3">
+        <v>3.9136299999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D113">
         <v>3</v>
       </c>
@@ -11570,10 +11644,10 @@
         <v>3</v>
       </c>
       <c r="H113">
-        <v>3.83114</v>
-      </c>
-    </row>
-    <row r="114" spans="4:8" x14ac:dyDescent="0.3">
+        <v>3.8270200000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D114">
         <v>3.25</v>
       </c>
@@ -11584,10 +11658,10 @@
         <v>3.25</v>
       </c>
       <c r="H114">
-        <v>3.7361300000000002</v>
-      </c>
-    </row>
-    <row r="115" spans="4:8" x14ac:dyDescent="0.3">
+        <v>3.74125</v>
+      </c>
+    </row>
+    <row r="115" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D115">
         <v>3.5</v>
       </c>
@@ -11598,10 +11672,10 @@
         <v>3.5</v>
       </c>
       <c r="H115">
-        <v>3.6442100000000002</v>
-      </c>
-    </row>
-    <row r="116" spans="4:8" x14ac:dyDescent="0.3">
+        <v>3.6574300000000002</v>
+      </c>
+    </row>
+    <row r="116" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D116">
         <v>3.75</v>
       </c>
@@ -11612,10 +11686,10 @@
         <v>3.75</v>
       </c>
       <c r="H116">
-        <v>3.5629599999999999</v>
-      </c>
-    </row>
-    <row r="117" spans="4:8" x14ac:dyDescent="0.3">
+        <v>3.5766399999999998</v>
+      </c>
+    </row>
+    <row r="117" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D117">
         <v>4</v>
       </c>
@@ -11629,7 +11703,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="118" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D118">
         <v>4.25</v>
       </c>
@@ -11640,10 +11714,10 @@
         <v>4.25</v>
       </c>
       <c r="H118">
-        <v>3.4490400000000001</v>
-      </c>
-    </row>
-    <row r="119" spans="4:8" x14ac:dyDescent="0.3">
+        <v>3.4331499999999999</v>
+      </c>
+    </row>
+    <row r="119" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D119">
         <v>4.5</v>
       </c>
@@ -11657,7 +11731,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="120" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D120">
         <v>4.75</v>
       </c>
@@ -11668,10 +11742,133 @@
         <v>4.75</v>
       </c>
       <c r="H120">
-        <v>3.63462</v>
-      </c>
-    </row>
-    <row r="121" spans="4:8" x14ac:dyDescent="0.3">
+        <v>3.6513</v>
+      </c>
+      <c r="L120">
+        <v>0</v>
+      </c>
+      <c r="M120">
+        <v>0.25</v>
+      </c>
+      <c r="N120">
+        <v>0.5</v>
+      </c>
+      <c r="O120">
+        <v>0.75</v>
+      </c>
+      <c r="P120">
+        <v>1</v>
+      </c>
+      <c r="Q120">
+        <v>1.25</v>
+      </c>
+      <c r="R120">
+        <v>1.5</v>
+      </c>
+      <c r="S120">
+        <v>1.75</v>
+      </c>
+      <c r="T120">
+        <v>2</v>
+      </c>
+      <c r="U120">
+        <v>2.25</v>
+      </c>
+      <c r="V120">
+        <v>2.5</v>
+      </c>
+      <c r="W120">
+        <v>2.75</v>
+      </c>
+      <c r="X120">
+        <v>3</v>
+      </c>
+      <c r="Y120">
+        <v>3.25</v>
+      </c>
+      <c r="Z120">
+        <v>3.5</v>
+      </c>
+      <c r="AA120">
+        <v>3.75</v>
+      </c>
+      <c r="AB120">
+        <v>4</v>
+      </c>
+      <c r="AC120">
+        <v>4.25</v>
+      </c>
+      <c r="AD120">
+        <v>4.5</v>
+      </c>
+      <c r="AE120">
+        <v>4.75</v>
+      </c>
+      <c r="AF120">
+        <v>5</v>
+      </c>
+      <c r="AG120">
+        <v>5.25</v>
+      </c>
+      <c r="AH120">
+        <v>5.5</v>
+      </c>
+      <c r="AI120">
+        <v>5.75</v>
+      </c>
+      <c r="AJ120">
+        <v>6</v>
+      </c>
+      <c r="AK120">
+        <v>6.25</v>
+      </c>
+      <c r="AL120">
+        <v>6.5</v>
+      </c>
+      <c r="AM120">
+        <v>6.75</v>
+      </c>
+      <c r="AN120">
+        <v>7</v>
+      </c>
+      <c r="AO120">
+        <v>7.25</v>
+      </c>
+      <c r="AP120">
+        <v>7.5</v>
+      </c>
+      <c r="AQ120">
+        <v>7.75</v>
+      </c>
+      <c r="AR120">
+        <v>8</v>
+      </c>
+      <c r="AS120">
+        <v>8.25</v>
+      </c>
+      <c r="AT120">
+        <v>8.5</v>
+      </c>
+      <c r="AU120">
+        <v>8.75</v>
+      </c>
+      <c r="AV120">
+        <v>9</v>
+      </c>
+      <c r="AW120">
+        <v>9.25</v>
+      </c>
+      <c r="AX120">
+        <v>9.5</v>
+      </c>
+      <c r="AY120">
+        <v>9.75</v>
+      </c>
+      <c r="AZ120">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D121">
         <v>5</v>
       </c>
@@ -11682,10 +11879,10 @@
         <v>5</v>
       </c>
       <c r="H121">
-        <v>4.2897800000000004</v>
-      </c>
-    </row>
-    <row r="122" spans="4:8" x14ac:dyDescent="0.3">
+        <v>4.2935999999999996</v>
+      </c>
+    </row>
+    <row r="122" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D122">
         <v>5.25</v>
       </c>
@@ -11696,10 +11893,10 @@
         <v>5.25</v>
       </c>
       <c r="H122">
-        <v>5.1500500000000002</v>
-      </c>
-    </row>
-    <row r="123" spans="4:8" x14ac:dyDescent="0.3">
+        <v>5.1391099999999996</v>
+      </c>
+    </row>
+    <row r="123" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D123">
         <v>5.5</v>
       </c>
@@ -11713,7 +11910,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D124">
         <v>5.75</v>
       </c>
@@ -11724,10 +11921,10 @@
         <v>5.75</v>
       </c>
       <c r="H124">
-        <v>6.6895100000000003</v>
-      </c>
-    </row>
-    <row r="125" spans="4:8" x14ac:dyDescent="0.3">
+        <v>6.6988799999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D125">
         <v>6</v>
       </c>
@@ -11741,7 +11938,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="126" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D126">
         <v>6.25</v>
       </c>
@@ -11752,10 +11949,10 @@
         <v>6.25</v>
       </c>
       <c r="H126">
-        <v>7.29643</v>
-      </c>
-    </row>
-    <row r="127" spans="4:8" x14ac:dyDescent="0.3">
+        <v>7.2929199999999996</v>
+      </c>
+    </row>
+    <row r="127" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D127">
         <v>6.5</v>
       </c>
@@ -11766,10 +11963,10 @@
         <v>6.5</v>
       </c>
       <c r="H127">
-        <v>7.4590699999999996</v>
-      </c>
-    </row>
-    <row r="128" spans="4:8" x14ac:dyDescent="0.3">
+        <v>7.4537800000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="4:52" x14ac:dyDescent="0.3">
       <c r="D128">
         <v>6.75</v>
       </c>
@@ -11780,7 +11977,7 @@
         <v>6.75</v>
       </c>
       <c r="H128">
-        <v>7.5928300000000002</v>
+        <v>7.58711</v>
       </c>
     </row>
     <row r="129" spans="4:8" x14ac:dyDescent="0.3">
@@ -11794,7 +11991,7 @@
         <v>7</v>
       </c>
       <c r="H129">
-        <v>7.70261</v>
+        <v>7.6974600000000004</v>
       </c>
     </row>
     <row r="130" spans="4:8" x14ac:dyDescent="0.3">
@@ -11808,7 +12005,7 @@
         <v>7.25</v>
       </c>
       <c r="H130">
-        <v>7.79331</v>
+        <v>7.78939</v>
       </c>
     </row>
     <row r="131" spans="4:8" x14ac:dyDescent="0.3">
@@ -11822,7 +12019,7 @@
         <v>7.5</v>
       </c>
       <c r="H131">
-        <v>7.8698399999999999</v>
+        <v>7.8674200000000001</v>
       </c>
     </row>
     <row r="132" spans="4:8" x14ac:dyDescent="0.3">
@@ -11836,7 +12033,7 @@
         <v>7.75</v>
       </c>
       <c r="H132">
-        <v>7.9371</v>
+        <v>7.9361100000000002</v>
       </c>
     </row>
     <row r="133" spans="4:8" x14ac:dyDescent="0.3">
@@ -11864,7 +12061,7 @@
         <v>8.25</v>
       </c>
       <c r="H134">
-        <v>8.0623799999999992</v>
+        <v>8.0628899999999994</v>
       </c>
     </row>
     <row r="135" spans="4:8" x14ac:dyDescent="0.3">
@@ -11878,7 +12075,7 @@
         <v>8.5</v>
       </c>
       <c r="H135">
-        <v>8.1248299999999993</v>
+        <v>8.1255699999999997</v>
       </c>
     </row>
     <row r="136" spans="4:8" x14ac:dyDescent="0.3">
@@ -11892,7 +12089,7 @@
         <v>8.75</v>
       </c>
       <c r="H136">
-        <v>8.1873199999999997</v>
+        <v>8.1880900000000008</v>
       </c>
     </row>
     <row r="137" spans="4:8" x14ac:dyDescent="0.3">
@@ -11906,7 +12103,7 @@
         <v>9</v>
       </c>
       <c r="H137">
-        <v>8.2498500000000003</v>
+        <v>8.2505100000000002</v>
       </c>
     </row>
     <row r="138" spans="4:8" x14ac:dyDescent="0.3">
@@ -11920,7 +12117,7 @@
         <v>9.25</v>
       </c>
       <c r="H138">
-        <v>8.3123900000000006</v>
+        <v>8.3128600000000006</v>
       </c>
     </row>
     <row r="139" spans="4:8" x14ac:dyDescent="0.3">
@@ -11934,7 +12131,7 @@
         <v>9.5</v>
       </c>
       <c r="H139">
-        <v>8.3749400000000005</v>
+        <v>8.3751899999999999</v>
       </c>
     </row>
     <row r="140" spans="4:8" x14ac:dyDescent="0.3">
@@ -11948,7 +12145,7 @@
         <v>9.75</v>
       </c>
       <c r="H140">
-        <v>8.4374800000000008</v>
+        <v>8.4375599999999995</v>
       </c>
     </row>
     <row r="141" spans="4:8" x14ac:dyDescent="0.3">

</xml_diff>